<commit_message>
Update dashboard for the second time
</commit_message>
<xml_diff>
--- a/dataset/Đơn vị các cột.xlsx
+++ b/dataset/Đơn vị các cột.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK1_2025\Data_Visualization\Final-Visualization\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TQHDL_final\Final-Visualization\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8E626-89A1-4A87-82D6-A513AD843DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,21 +520,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="194.109375" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="194.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -543,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -551,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -559,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -567,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -583,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -591,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -599,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -607,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -615,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -623,7 +622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -631,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -639,7 +638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -647,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -655,7 +654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -663,7 +662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -671,7 +670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -679,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -687,7 +686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -695,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -703,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -712,7 +711,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -720,7 +719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -728,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -736,7 +735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -744,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -752,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -760,7 +759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
@@ -768,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -776,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -784,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
@@ -792,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -800,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
@@ -808,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
@@ -816,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -824,7 +823,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>

</xml_diff>